<commit_message>
Merge, Doku, neues SQL login + neuer DB name
</commit_message>
<xml_diff>
--- a/Doku/GanttDiagramm..xlsx
+++ b/Doku/GanttDiagramm..xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12000" windowHeight="2565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="2565"/>
   </bookViews>
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
@@ -624,56 +624,12 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -685,10 +641,19 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,7 +661,44 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
@@ -1005,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:C50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:Z52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1040,7 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="80" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="19"/>
@@ -1047,36 +1049,36 @@
         <v>5</v>
       </c>
       <c r="F1" s="23"/>
-      <c r="G1" s="80">
+      <c r="G1" s="91">
         <v>9.01</v>
       </c>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="80">
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="91">
         <v>10.01</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="80">
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="91">
         <v>16.010000000000002</v>
       </c>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="80">
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="91">
         <v>17.010000000000002</v>
       </c>
-      <c r="T1" s="81"/>
-      <c r="U1" s="81"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="80">
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="91">
         <v>23.01</v>
       </c>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="81"/>
-      <c r="Z1" s="82"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="93"/>
       <c r="AA1"/>
       <c r="AB1"/>
       <c r="AC1"/>
@@ -1146,7 +1148,7 @@
       <c r="CO1"/>
     </row>
     <row r="2" spans="1:93" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
+      <c r="B2" s="80"/>
       <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
@@ -1284,19 +1286,19 @@
       <c r="CO2"/>
     </row>
     <row r="3" spans="1:93" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="91">
+      <c r="B3" s="76">
         <v>1</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="73"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="38" t="s">
         <v>19</v>
       </c>
@@ -1380,11 +1382,11 @@
       <c r="CO3"/>
     </row>
     <row r="4" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="88"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
       <c r="F4" s="39" t="s">
         <v>20</v>
       </c>
@@ -1468,11 +1470,11 @@
       <c r="CO4"/>
     </row>
     <row r="5" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
       <c r="F5" s="39" t="s">
         <v>21</v>
       </c>
@@ -1556,11 +1558,11 @@
       <c r="CO5"/>
     </row>
     <row r="6" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
       <c r="F6" s="40" t="s">
         <v>22</v>
       </c>
@@ -1653,17 +1655,17 @@
       <c r="CO6"/>
     </row>
     <row r="7" spans="1:93" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="76">
         <v>2</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="86"/>
       <c r="F7" s="26" t="s">
         <v>19</v>
       </c>
@@ -1747,11 +1749,11 @@
       <c r="CO7"/>
     </row>
     <row r="8" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="76"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="87"/>
       <c r="F8" s="33" t="s">
         <v>20</v>
       </c>
@@ -1835,11 +1837,11 @@
       <c r="CO8"/>
     </row>
     <row r="9" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="88"/>
-      <c r="B9" s="91"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="76"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="33" t="s">
         <v>21</v>
       </c>
@@ -1920,11 +1922,11 @@
       <c r="CO9"/>
     </row>
     <row r="10" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="88"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="78"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="27" t="s">
         <v>24</v>
       </c>
@@ -2017,15 +2019,15 @@
       <c r="CO10"/>
     </row>
     <row r="11" spans="1:93" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="88"/>
-      <c r="B11" s="92">
+      <c r="A11" s="74"/>
+      <c r="B11" s="81">
         <v>3</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="73"/>
-      <c r="E11" s="74"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="26" t="s">
         <v>19</v>
       </c>
@@ -2109,11 +2111,11 @@
       <c r="CO11"/>
     </row>
     <row r="12" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="88"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="76"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="33" t="s">
         <v>20</v>
       </c>
@@ -2195,11 +2197,11 @@
       <c r="CO12"/>
     </row>
     <row r="13" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="88"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="76"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="87"/>
       <c r="F13" s="33" t="s">
         <v>21</v>
       </c>
@@ -2281,11 +2283,11 @@
       <c r="CO13"/>
     </row>
     <row r="14" spans="1:93" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="88"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="78"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="88"/>
       <c r="F14" s="27" t="s">
         <v>24</v>
       </c>
@@ -2367,13 +2369,13 @@
       <c r="CO14"/>
     </row>
     <row r="15" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="88"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="48"/>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="74"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="86"/>
       <c r="F15" s="26" t="s">
         <v>19</v>
       </c>
@@ -2466,11 +2468,11 @@
       <c r="CO15"/>
     </row>
     <row r="16" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="88"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="48"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="76"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="87"/>
       <c r="F16" s="33" t="s">
         <v>20</v>
       </c>
@@ -2552,11 +2554,11 @@
       <c r="CO16"/>
     </row>
     <row r="17" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="48"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="76"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="87"/>
       <c r="F17" s="33" t="s">
         <v>21</v>
       </c>
@@ -2641,11 +2643,11 @@
       <c r="CO17"/>
     </row>
     <row r="18" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="48"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="78"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="88"/>
       <c r="F18" s="27" t="s">
         <v>24</v>
       </c>
@@ -2738,13 +2740,13 @@
       <c r="CO18"/>
     </row>
     <row r="19" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="48"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="74"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="86"/>
       <c r="F19" s="26" t="s">
         <v>19</v>
       </c>
@@ -2837,11 +2839,11 @@
       <c r="CO19"/>
     </row>
     <row r="20" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="48"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="76"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="87"/>
       <c r="F20" s="33" t="s">
         <v>20</v>
       </c>
@@ -2924,11 +2926,11 @@
       <c r="CO20"/>
     </row>
     <row r="21" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="48"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="76"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="87"/>
       <c r="F21" s="33" t="s">
         <v>21</v>
       </c>
@@ -3010,11 +3012,11 @@
       <c r="CO21"/>
     </row>
     <row r="22" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="88"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="48"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="78"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="88"/>
       <c r="F22" s="27" t="s">
         <v>24</v>
       </c>
@@ -3107,13 +3109,13 @@
       <c r="CO22"/>
     </row>
     <row r="23" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="88"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="48"/>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="73"/>
-      <c r="E23" s="74"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="86"/>
       <c r="F23" s="26" t="s">
         <v>19</v>
       </c>
@@ -3206,11 +3208,11 @@
       <c r="CO23"/>
     </row>
     <row r="24" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="88"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="48"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="76"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="87"/>
       <c r="F24" s="33" t="s">
         <v>20</v>
       </c>
@@ -3292,11 +3294,11 @@
       <c r="CO24"/>
     </row>
     <row r="25" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="48"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="76"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="87"/>
       <c r="F25" s="33" t="s">
         <v>21</v>
       </c>
@@ -3379,11 +3381,11 @@
       <c r="CO25"/>
     </row>
     <row r="26" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="50"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="88"/>
       <c r="F26" s="27" t="s">
         <v>24</v>
       </c>
@@ -3476,15 +3478,15 @@
       <c r="CO26"/>
     </row>
     <row r="27" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="70" t="s">
+      <c r="C27" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="73"/>
-      <c r="E27" s="74"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="86"/>
       <c r="F27" s="26" t="s">
         <v>19</v>
       </c>
@@ -3577,11 +3579,11 @@
       <c r="CO27"/>
     </row>
     <row r="28" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="50"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="76"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="87"/>
       <c r="F28" s="33" t="s">
         <v>20</v>
       </c>
@@ -3674,11 +3676,11 @@
       <c r="CO28"/>
     </row>
     <row r="29" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="88"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="50"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="76"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="87"/>
       <c r="F29" s="33" t="s">
         <v>21</v>
       </c>
@@ -3771,11 +3773,11 @@
       <c r="CO29"/>
     </row>
     <row r="30" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="88"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="50"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="78"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="88"/>
       <c r="F30" s="33" t="s">
         <v>24</v>
       </c>
@@ -3868,13 +3870,13 @@
       <c r="CO30"/>
     </row>
     <row r="31" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="50"/>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="73"/>
-      <c r="E31" s="74"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="86"/>
       <c r="F31" s="26" t="s">
         <v>19</v>
       </c>
@@ -3967,11 +3969,11 @@
       <c r="CO31"/>
     </row>
     <row r="32" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="50"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="76"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="87"/>
       <c r="F32" s="33" t="s">
         <v>20</v>
       </c>
@@ -4064,11 +4066,11 @@
       <c r="CO32"/>
     </row>
     <row r="33" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="88"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="76"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="87"/>
       <c r="F33" s="33" t="s">
         <v>21</v>
       </c>
@@ -4161,11 +4163,11 @@
       <c r="CO33"/>
     </row>
     <row r="34" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="88"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="50"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="78"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="88"/>
       <c r="F34" s="27" t="s">
         <v>24</v>
       </c>
@@ -4258,13 +4260,13 @@
       <c r="CO34"/>
     </row>
     <row r="35" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="88"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="50"/>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="73"/>
-      <c r="E35" s="74"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="86"/>
       <c r="F35" s="26" t="s">
         <v>19</v>
       </c>
@@ -4357,11 +4359,11 @@
       <c r="CO35"/>
     </row>
     <row r="36" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="88"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="50"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="76"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="87"/>
       <c r="F36" s="33" t="s">
         <v>20</v>
       </c>
@@ -4454,11 +4456,11 @@
       <c r="CO36"/>
     </row>
     <row r="37" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="88"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="50"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="76"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="87"/>
       <c r="F37" s="33" t="s">
         <v>21</v>
       </c>
@@ -4551,11 +4553,11 @@
       <c r="CO37"/>
     </row>
     <row r="38" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="89"/>
+      <c r="A38" s="75"/>
       <c r="B38" s="50"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="78"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="88"/>
       <c r="F38" s="27" t="s">
         <v>24</v>
       </c>
@@ -4650,11 +4652,11 @@
     <row r="39" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
       <c r="B39" s="50"/>
-      <c r="C39" s="70" t="s">
+      <c r="C39" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="74"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="86"/>
       <c r="F39" s="26" t="s">
         <v>19</v>
       </c>
@@ -4749,9 +4751,9 @@
     <row r="40" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
       <c r="B40" s="50"/>
-      <c r="C40" s="71"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="76"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="87"/>
       <c r="F40" s="33" t="s">
         <v>20</v>
       </c>
@@ -4846,9 +4848,9 @@
     <row r="41" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49"/>
       <c r="B41" s="50"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="76"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="87"/>
       <c r="F41" s="33" t="s">
         <v>21</v>
       </c>
@@ -4943,9 +4945,9 @@
     <row r="42" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
       <c r="B42" s="50"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="78"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="88"/>
       <c r="F42" s="27" t="s">
         <v>24</v>
       </c>
@@ -4959,7 +4961,7 @@
       <c r="N42" s="14"/>
       <c r="O42" s="12"/>
       <c r="P42" s="13"/>
-      <c r="Q42" s="94"/>
+      <c r="Q42" s="70"/>
       <c r="R42" s="14"/>
       <c r="S42" s="65"/>
       <c r="T42" s="18"/>
@@ -5038,19 +5040,19 @@
       <c r="CO42"/>
     </row>
     <row r="43" spans="1:93" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="87" t="s">
+      <c r="A43" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="91">
+      <c r="B43" s="76">
         <v>5</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="73" t="s">
+      <c r="D43" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="74"/>
+      <c r="E43" s="86"/>
       <c r="F43" s="26" t="s">
         <v>19</v>
       </c>
@@ -5064,8 +5066,10 @@
       <c r="T43" s="67"/>
       <c r="U43" s="67"/>
       <c r="V43" s="11"/>
-      <c r="W43" s="9"/>
-      <c r="Z43" s="11"/>
+      <c r="W43" s="60"/>
+      <c r="X43" s="17"/>
+      <c r="Y43" s="17"/>
+      <c r="Z43" s="59"/>
       <c r="AA43"/>
       <c r="AB43"/>
       <c r="AC43"/>
@@ -5135,11 +5139,11 @@
       <c r="CO43"/>
     </row>
     <row r="44" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="91"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="76"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="87"/>
       <c r="F44" s="33" t="s">
         <v>20</v>
       </c>
@@ -5149,8 +5153,10 @@
       <c r="R44" s="14"/>
       <c r="S44" s="12"/>
       <c r="V44" s="14"/>
-      <c r="W44" s="12"/>
-      <c r="Z44" s="14"/>
+      <c r="W44" s="95"/>
+      <c r="X44" s="68"/>
+      <c r="Y44" s="68"/>
+      <c r="Z44" s="96"/>
       <c r="AA44"/>
       <c r="AB44"/>
       <c r="AC44"/>
@@ -5220,11 +5226,11 @@
       <c r="CO44"/>
     </row>
     <row r="45" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="88"/>
-      <c r="B45" s="91"/>
-      <c r="C45" s="71"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="76"/>
+      <c r="A45" s="74"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="87"/>
       <c r="F45" s="33" t="s">
         <v>21</v>
       </c>
@@ -5234,8 +5240,10 @@
       <c r="R45" s="14"/>
       <c r="S45" s="12"/>
       <c r="V45" s="14"/>
-      <c r="W45" s="12"/>
-      <c r="Z45" s="14"/>
+      <c r="W45" s="62"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="61"/>
       <c r="AA45"/>
       <c r="AB45"/>
       <c r="AC45"/>
@@ -5305,11 +5313,11 @@
       <c r="CO45"/>
     </row>
     <row r="46" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="89"/>
-      <c r="B46" s="91"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="78"/>
+      <c r="A46" s="75"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="85"/>
+      <c r="E46" s="88"/>
       <c r="F46" s="27" t="s">
         <v>24</v>
       </c>
@@ -5329,10 +5337,10 @@
       <c r="T46" s="13"/>
       <c r="U46" s="13"/>
       <c r="V46" s="14"/>
-      <c r="W46" s="12"/>
-      <c r="X46" s="13"/>
-      <c r="Y46" s="13"/>
-      <c r="Z46" s="14"/>
+      <c r="W46" s="65"/>
+      <c r="X46" s="18"/>
+      <c r="Y46" s="18"/>
+      <c r="Z46" s="63"/>
       <c r="AA46"/>
       <c r="AB46"/>
       <c r="AC46"/>
@@ -5402,17 +5410,17 @@
       <c r="CO46"/>
     </row>
     <row r="47" spans="1:93" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="91">
+      <c r="B47" s="76">
         <v>6</v>
       </c>
-      <c r="C47" s="70" t="s">
+      <c r="C47" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="73"/>
-      <c r="E47" s="74"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="86"/>
       <c r="F47" s="26" t="s">
         <v>19</v>
       </c>
@@ -5494,11 +5502,11 @@
       <c r="CO47"/>
     </row>
     <row r="48" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="88"/>
-      <c r="B48" s="91"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="76"/>
+      <c r="A48" s="74"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="87"/>
       <c r="F48" s="33" t="s">
         <v>20</v>
       </c>
@@ -5579,11 +5587,11 @@
       <c r="CO48"/>
     </row>
     <row r="49" spans="1:93" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="88"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="76"/>
+      <c r="A49" s="74"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="87"/>
       <c r="F49" s="33" t="s">
         <v>21</v>
       </c>
@@ -5664,11 +5672,11 @@
       <c r="CO49"/>
     </row>
     <row r="50" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="89"/>
-      <c r="B50" s="91"/>
-      <c r="C50" s="72"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="78"/>
+      <c r="A50" s="75"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="88"/>
       <c r="F50" s="27" t="s">
         <v>24</v>
       </c>
@@ -5761,15 +5769,15 @@
       <c r="CO50"/>
     </row>
     <row r="51" spans="1:93" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="83"/>
-      <c r="B51" s="79">
+      <c r="A51" s="71"/>
+      <c r="B51" s="94">
         <v>11</v>
       </c>
-      <c r="C51" s="83" t="s">
+      <c r="C51" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
       <c r="F51" s="28"/>
       <c r="G51" s="29"/>
       <c r="H51" s="30"/>
@@ -5860,11 +5868,11 @@
       <c r="CO51"/>
     </row>
     <row r="52" spans="1:93" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="84"/>
-      <c r="B52" s="79"/>
-      <c r="C52" s="84"/>
-      <c r="D52" s="86"/>
-      <c r="E52" s="86"/>
+      <c r="A52" s="72"/>
+      <c r="B52" s="94"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="90"/>
+      <c r="E52" s="90"/>
       <c r="F52" s="55"/>
       <c r="G52" s="56"/>
       <c r="H52" s="57"/>
@@ -5956,12 +5964,29 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="D3:E6"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:E52"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="D19:E22"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="D23:E26"/>
+    <mergeCell ref="D27:E30"/>
+    <mergeCell ref="D35:E38"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="D11:E14"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:E34"/>
+    <mergeCell ref="C39:C42"/>
     <mergeCell ref="A7:A38"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B1:B2"/>
@@ -5976,29 +6001,12 @@
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:E6"/>
-    <mergeCell ref="D47:E50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:E52"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D43:E46"/>
-    <mergeCell ref="D19:E22"/>
-    <mergeCell ref="D15:E18"/>
-    <mergeCell ref="D23:E26"/>
-    <mergeCell ref="D27:E30"/>
-    <mergeCell ref="D35:E38"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="D11:E14"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:E34"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:E42"/>
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="B43:B46"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>